<commit_message>
8-7 update; after progress meeting with Will
</commit_message>
<xml_diff>
--- a/Screen Sheets/Data/Antibiotic_Screen.xlsx
+++ b/Screen Sheets/Data/Antibiotic_Screen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bubba\Ludington Lab Internship\Screen Sheets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01E597D-FDFF-41DD-8AFF-008C269C9E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B103DA95-5B78-4571-99C6-0EF4B54360F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{6E9D2C87-4445-4FA7-A0ED-A44CFD788CA0}"/>
   </bookViews>
@@ -435,10 +435,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -446,12 +460,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,14 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1562,7 +1562,7 @@
   <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,23 +1585,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="9"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1625,124 +1625,124 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="8">
         <v>2.444</v>
       </c>
       <c r="E4" s="5">
         <v>42.761000000000003</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="8">
         <v>0.88700000000000001</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="19">
+      <c r="G4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="8">
         <v>1.0960000000000001</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="8">
         <v>3.7480000000000002</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="8">
         <v>320.702</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="8">
         <v>4.9550000000000001</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="9" t="s">
         <v>69</v>
       </c>
       <c r="H5" s="5">
         <v>6.0579999999999998</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="8">
         <v>0.54900000000000004</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="5">
         <v>16.329000000000001</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="20">
+      <c r="E6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="9">
         <v>2.0840000000000001</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="8">
         <v>3.391</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="8">
         <v>2.2429999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="8">
         <v>32.363</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="5">
         <v>0.52300000000000002</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="19">
+      <c r="F7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="8">
         <v>5.7229999999999999</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="8">
         <v>2.3140000000000001</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="9" t="s">
         <v>69</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1751,18 +1751,18 @@
       <c r="G8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="19">
+      <c r="H8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="8">
         <v>4.3570000000000002</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="8">
         <v>0.97199999999999998</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1772,31 +1772,31 @@
       <c r="E9" s="5">
         <v>0.36899999999999999</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="9">
         <v>4.8730000000000002</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="19">
+      <c r="G9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="8">
         <v>1.073</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="8">
         <v>0.94599999999999995</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="9" t="s">
         <v>69</v>
       </c>
       <c r="F10" s="7"/>
@@ -1806,101 +1806,102 @@
       <c r="J10" s="7"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="2:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B13:G14"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="B4:B10"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="C18:G18"/>
-    <mergeCell ref="B13:G14"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="B4:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>